<commit_message>
Report and Glossary update + AnalyzerServiceTest typos correction
</commit_message>
<xml_diff>
--- a/LanguageDetectionPrototype/Documents/Glossary.xlsx
+++ b/LanguageDetectionPrototype/Documents/Glossary.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\inesc\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\inesc\Desktop\Projetos Git\DuckSoftWorks\DuckSoftWorks\LanguageDetectionPrototype\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B06C845C-CB6F-4277-8641-31F1FA1C07A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1FE70AD-809E-4238-90A0-B7EEB7E1F1E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{235FC9EE-D9E3-49E6-95E0-C435C389101B}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="43">
   <si>
     <t>Acronym</t>
   </si>
@@ -154,6 +154,24 @@
   </si>
   <si>
     <t>Lucene is a Java library providing powerful indexing and search features, as well as spellchecking, hit highlighting and advanced analysis/tokenization capabilities.</t>
+  </si>
+  <si>
+    <t>PT</t>
+  </si>
+  <si>
+    <t>EN</t>
+  </si>
+  <si>
+    <t>ES</t>
+  </si>
+  <si>
+    <t>Portuguese</t>
+  </si>
+  <si>
+    <t>English</t>
+  </si>
+  <si>
+    <t>Spanish</t>
   </si>
 </sst>
 </file>
@@ -240,8 +258,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{90C6256B-FEC0-4BA3-85F4-0D6DF0FDF16B}" name="Table1" displayName="Table1" ref="A1:C17" totalsRowShown="0">
-  <autoFilter ref="A1:C17" xr:uid="{90C6256B-FEC0-4BA3-85F4-0D6DF0FDF16B}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{90C6256B-FEC0-4BA3-85F4-0D6DF0FDF16B}" name="Table1" displayName="Table1" ref="A1:C20" totalsRowShown="0">
+  <autoFilter ref="A1:C20" xr:uid="{90C6256B-FEC0-4BA3-85F4-0D6DF0FDF16B}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C17">
     <sortCondition ref="B1:B17"/>
   </sortState>
@@ -551,10 +569,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1225BEF3-676C-4E24-8737-736631426F25}">
-  <dimension ref="A1:C17"/>
+  <dimension ref="A1:C20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -709,10 +727,35 @@
         <v>23</v>
       </c>
     </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>